<commit_message>
[Feat] Add Player Scripts
- MVC 모델을 적용 함
- 컨트롤러는 상태 패턴을 적용
- 상태 패턴을 위해 Base State, State Machine, Player State 스크립트 생성
</commit_message>
<xml_diff>
--- a/Project_Design/Features.xlsx
+++ b/Project_Design/Features.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ttangu\바탕 화면\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ttangu\바탕 화면\xrp\Unity\ProjectZ\Project_Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4308B4A-55A8-4353-894F-E62BF803242A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28B304B6-CF2A-44B3-8E90-510D2B510179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2180" yWindow="820" windowWidth="35700" windowHeight="20570" activeTab="2" xr2:uid="{4CF35248-9F94-4C5D-AC8E-122F6CBF2D14}"/>
+    <workbookView xWindow="1400" yWindow="530" windowWidth="35700" windowHeight="20570" activeTab="4" xr2:uid="{4CF35248-9F94-4C5D-AC8E-122F6CBF2D14}"/>
   </bookViews>
   <sheets>
     <sheet name="필요 기능 모음" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="350">
   <si>
     <t>조작 키 (인풋시스템) - C버튼 생략. 다른 키들로 대체함</t>
   </si>
@@ -245,30 +245,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>구르는 상태</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>새총 조준 상태</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>새총 아이템 선택 후 조준 키</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>대화 상태</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>대화 시 조작 불능</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>대화 시 대화 주체들을 기준으로 카메라 잡힘(시네머신 기능 중에 있음)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>주목 이동상태</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -277,22 +257,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>A키 누르면 낙하</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>올라가면 전용 애니메이션</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>올라가는 전용 애니메이션</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>올라가는 자세 애니메이션</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>내려가는 자세 애니메이션</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -301,10 +265,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>캐릭터와 Y좌표 판단을 해서, 올라갈 수 있는 높이면 매달림</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>조작키 입력시 이동상태로 변경</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -321,22 +281,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>조작키로 낙하 지점 조정 가능(이동속도 절반)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>공격 키 입력 시, 점프 공격상태로 전환</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이동 키 입력이 진행방향과 일치하면 조금 더 빠르게 구른다((Vertical 값 +1)*moveSpeed을 하면 딱 맞음)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주목키를 풀면 아이들 상태</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>공격 시간 끝나면 아이들 상태</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -465,18 +409,6 @@
     <t>→</t>
   </si>
   <si>
-    <t>점프상태</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>물건 집은 상태</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이동 및 주목 상태 가능</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Z</t>
   </si>
   <si>
@@ -510,10 +442,6 @@
     <t>노란색은 픽스 (내가 제시한 조작키 기준으로)</t>
   </si>
   <si>
-    <t>기어가는 상태</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>끝까지 기어가면 다음 씬으로 전환(기어가는 중에 전환됨)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -535,10 +463,6 @@
     <t>새총 A로 조준하면서 S로 샷</t>
   </si>
   <si>
-    <t>물상태</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>잠수상태</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -551,14 +475,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>물에서 벗어나는 상태(지면이 있을 시)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>캐릭터와 지면의 y좌표 차이로 판단</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>부모상태</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -567,22 +483,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>박스 이동 상태</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>박스 근처에서 박스 방향으로 A키를 눌러 이동상태에서 전환</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A키를 떼면은 아이들상태로 전환</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A키를 누른 상태에서 이동방향으로 누르면 상자와 함께 이동</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1인칭 모드는 알아서... ㅋㅋㅋㅋㅋㅋㅋㅋㅋㅋㅋㅋㅋㅋ</t>
   </si>
   <si>
@@ -630,10 +530,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>어떤 상태이든 피격 상태로 전환 가능</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>이름</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -758,10 +654,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>모든 공격은 3연타</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>회전베기</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -786,10 +678,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>무기 소지 안한 상태로 A키 - 구르기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>주목 아이들 상태</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -798,10 +686,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>좌우 키 입력은 게걸음, 방향키에 맞게 A 키 누를 시 점프함 -&gt; 좌,우 - 좌우뛰기, 뒤 - 백덤블링</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>공격상태 동안은 조작키가 먹지 않음. 각 공격 시간이 끝나면 Idle로 넘어감. 일정 시간 이내에 다시 공격 키 입력시 연속 타격으로 넘어감</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -826,10 +710,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>상호 작용 대상에게 지정 범위 안에서 A키</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>이동 키 입력 시 상 하 좌 우로 방어 각도 설정</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -842,14 +722,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>전진 공격 - 종베기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>일반 공격 - 횡베기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>전진 키 + 공격 키 (일정 시간 이내에 다시 입력하면 연속공격, 벗어나면 Idle)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -894,10 +766,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>이동 조작 키 입력, A 키 입력</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>이동 키</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -982,14 +850,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>벽을 탄 상태로 상하좌우 이동 가능</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이동 키 , A키</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>상 하 이동키 , A키</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -998,26 +858,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>탈 수 있는 벽 앞에서 전진 키 // 낙하 상태 중 OnCollision</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>탈 수 있는 사다리 앞에서 전진 키, A 키 // 낙하 상태 중 OnCollision</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>물의 수면 높이가 캐릭터 y 좌표와 비교해서 일정 높이 이상이면 물 상태 판정</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>타임스케일 =0, 무적</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이동 키, 공격 키</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>종베기</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1034,7 +878,513 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>일정 높이 이상에서 땅으로 떨어지면 체력 잃음(피격 상태 중 하나, 무적), 물로 떨어지면 물</t>
+    <t>상호작용이 종료되면 Idle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Idle, Move -&gt; 상호 작용 대상에게 지정 범위 안에서 A키</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Idle -&gt; 대상과 일정 거리 안에 있으면 A키</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대화창이 종료되면 Idle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>타임스케일 =0, 무적, 카메라가 두 물체를 중심으로 잡음(씨네머신 기능)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>레이캐스트로 IInteract 인터페이스를 검출한다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사운드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>뒤돌아가던지 앞으로 쭉 나아가면 Idle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대부분 A키로 상호작용한다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A키, 이동 키 중에서 Up키</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Move 상태로 접근할 경우 벽에 매달린 상태로 진입, 벽 판단 범위보다 긴 상태일 때 잡기 가능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A 키 입력 시 상호작용 가능 상황이면 상호작용 상태로 변경</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공격 시간 종료 후</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>낙하 상태 종료 후</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주목 상태를 풀 시(키 토글, 홀드 멈춤) -&gt; Idle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가만히 있으면 박스잡기 Idle, 움직이면 움직이는 곳으로 Move(앞 뒤만 가능)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>박스 이동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기어가기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>레이캐스트로 상호작용 거리 확인 , 상호작용 중에는 무적(박스제외)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이동 키 입력이 없을 시 &amp;&amp; A 키 홀드를 풀면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Idle -&gt; 대상과 일정 거리 안에 있으면 A키 홀드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Idamagable 피격 시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>낙하 피격</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>낙하 높이 차로 인한 피격</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>무기 발도 상태에서 A(이동키는 없어야 함)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전진 키 입력 &amp;&amp; A키 입력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구르기 시간 종료 후</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>백덤블링의 경우 낙하 상태, 전진 키의 경우 이동상태의 전진의 경우 논리를 전부 가져오면 됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">방향 키에 맞춰 이동 좌우는 게걸음 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>방향키와 함께 A 키 누를 시 점프함 -&gt; 좌,우 - 좌우뛰기, 뒤 - 백덤블링</t>
+  </si>
+  <si>
+    <t>이동 점프</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이동 조작 키</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이동 조작 키 &amp;&amp; A키</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이동 구르기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>구르는 중 키 입력 가능(상,하 키 입력값만 유효)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이동 키, A 키</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Idle -&gt; 레이캐스트 일정 범위 내에서 A키</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물건 집기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Idle상태에서 A키 -&gt; 내려놓기, Move 상태에서 A키 -&gt; 던지기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. 무언가 들고 있을 시 내려놓기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>중간에 A키 누르면 낙하 상태로 전이, 지상에 도달 시 아이들상태로 전환</t>
+  </si>
+  <si>
+    <t>Move -&gt; 레이캐스트 일정 범위 안(매우짧음)에 벽을 탈 수 있는 것이면 벽타기 상태 // 낙하 상태 중 OnCollision</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>무적 //이동 키 입력이 진행방향과 일치하면 조금 더 빠르게 구른다((Vertical 값 +1)*moveSpeed을 하면 딱 맞음)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물 상태</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>올라가기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>어떤 상태이든 피격 상태로 전환 가능 , 피격 대상 기준 뒤로 넉백이 있음(점프)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일반 공격 - 횡베기, 3연타 가능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전진 공격 - 종베기, 3연타 가능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>낙하 상태 -&gt; 일정 시간 후 피격 상태</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>피격 시간 종료 후</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>무적, 넉백없음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>무적, 넉백이 있음</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>탈 수 있는 사다리 앞에서 전진 키, Idle -&gt; A 키 // 낙하 상태 중 OnCollision</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일정 시간 이상 낙하해서 땅으로 떨어지면 체력 잃음(피격 상태, 무적), 낙하 시간 초기화 및 낙하 판정 false로 변경, 조작키로 낙하 지점 조정 가능(이동속도 절반), 중력가속도 영향 받음( 낙하속도 상한선있음), 낙하 시간을 업데이트마다 더함</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>땅이면 Idle, 물로 떨어지면 물 상태</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1인칭 상태</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5. 1인칭 변환</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R 스틱 클릭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>카메라 이동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R 스틱</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Idle -&gt; R스틱 클릭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R스틱 클릭, 취소 버튼 -&gt; Idle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>인벤토리</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스타트 키, 취소 키, A키</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Idle, Move -&gt; 스타트 키</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스타트키, 취소 키 -&gt; Idle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TimeScale = 0, 음악 소리 작아짐</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>내려가기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Up키</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Down키, A키</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>벽 상태 -&gt; 낙하</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>무적 아님, 집을 수 있는 것들은 Idamagable + Igrabbable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>대화, 조사 처럼 들어가는 걸로 처리, 사용할 아이템 선택 가능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주목 키</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">1인칭 -&gt; 새총 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이템이 새총인 상태에서 조준 키 홀드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>조준키 홀드 해제</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>아이템 사용 키(새총발사), 조준키</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A 키(잠수)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>캐릭터와 지면의 y좌표 차이로 판단, 레이캐스트(아래)로 일정 범위 이내일 시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이동 키 입력 시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이동 키 입력 종료 시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이동 키 ,A 키 홀드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물 아이들, 이동 -&gt; A 키 홀드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A키 홀드 해제 시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y좌표가 A 홀드 시간 만큼 감소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물 밑의 스위치와 상호작용 가능(스위치는 OnCollision 처리하면 됨)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잠수 상태에서 A키 홀드 해제시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>잠수 -&gt; 수면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y좌표가 수면위치까지 점차적 증가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>수면 복귀 시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5. 인풋시스템</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상호작용 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 나비 및 주목 시스템</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.1 나비는 주목 Position으로 날라감. 아닌 경우 되돌아옴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 물체 및 NPC와 상호작용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. 여러 상호작용 상태들 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>레벨 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. 마을의 방들</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. 씬전환 기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 에셋 배치</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 라이트 배치</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3. 라이트 맵 생성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>필요한 곳들에 효과음 이벤트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>플레이어를 쫒아오는 적 구현(NavMesh)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4. 필드 아이템 OnCollision 구현</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스크립터블 오브젝트</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CSV 또는 JSON</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 던전</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2. 마을</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>테스트 씬 구성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>필요한 모든 기능들을 테스트 할 수 있는 테스트 씬 구성</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>전투</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상호작용</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상태변경</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>물, 공중, 점프 등등</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>점프 상태</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이동 키 또는 구르기로 플랫폼 끄트머리(OnTrigger 얇은 범위) 입장 시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>낙하 상 태 종료 시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>점프 가능한 플랫폼에서 점프, 낙하 상태</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>점프 공격 가능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y 좌표가 감소하면서 낙하, 벽상태, 이동 -&gt; 점프 상태에서 넘어온 경우 전용 애니메이션</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>낙하 중 공격 키를 누르면 점프공격이 나간다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>다른 상태들 쪽에서 전이해서 들어온다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>낙하 중 공격 키 입력 시, 점프 공격상태로 전환</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모든 점프는 낙하 상태, 백덤블링은 점프공격으로 연결 안됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>무기 소지를 안하고 있어야 됨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이동 키 입력이 없을 시, 공격 시</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1125,14 +1475,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
@@ -1165,10 +1512,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1490,7 +1833,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3563BFD3-F5EB-4F57-BF3B-6CCD4CE1AEEB}">
   <dimension ref="A1:A34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
@@ -1504,167 +1849,167 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1675,143 +2020,252 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A167A73-9D4E-45A5-86A6-04054743346A}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="17.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.9140625" customWidth="1"/>
     <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>154</v>
+        <v>129</v>
       </c>
       <c r="B2" t="s">
-        <v>150</v>
+        <v>125</v>
       </c>
       <c r="C2" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="D2" t="s">
-        <v>162</v>
+        <v>136</v>
       </c>
       <c r="E2" t="s">
-        <v>163</v>
+        <v>137</v>
       </c>
       <c r="F2" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="G2" t="s">
-        <v>165</v>
+        <v>139</v>
       </c>
       <c r="H2" t="s">
-        <v>166</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
-        <v>151</v>
+        <v>126</v>
       </c>
       <c r="C3" t="s">
-        <v>179</v>
+        <v>153</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
-        <v>152</v>
+        <v>127</v>
       </c>
       <c r="C4" t="s">
-        <v>179</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
-        <v>153</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>155</v>
-      </c>
       <c r="B6" t="s">
-        <v>156</v>
-      </c>
-      <c r="C6" t="s">
-        <v>161</v>
-      </c>
-      <c r="D6" t="s">
-        <v>163</v>
-      </c>
-      <c r="E6" t="s">
-        <v>162</v>
+        <v>313</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>130</v>
+      </c>
       <c r="B7" t="s">
-        <v>157</v>
+        <v>131</v>
       </c>
       <c r="C7" t="s">
-        <v>174</v>
+        <v>135</v>
       </c>
       <c r="D7" t="s">
-        <v>175</v>
+        <v>137</v>
       </c>
       <c r="E7" t="s">
-        <v>176</v>
-      </c>
-      <c r="F7" t="s">
-        <v>177</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
-        <v>158</v>
+        <v>132</v>
       </c>
       <c r="C8" t="s">
-        <v>173</v>
+        <v>148</v>
       </c>
       <c r="D8" t="s">
-        <v>178</v>
+        <v>149</v>
+      </c>
+      <c r="E8" t="s">
+        <v>150</v>
+      </c>
+      <c r="F8" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>168</v>
-      </c>
       <c r="B9" t="s">
-        <v>169</v>
+        <v>133</v>
       </c>
       <c r="C9" t="s">
-        <v>170</v>
+        <v>147</v>
+      </c>
+      <c r="D9" t="s">
+        <v>152</v>
+      </c>
+      <c r="E9" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>142</v>
+      </c>
       <c r="B10" t="s">
-        <v>171</v>
+        <v>143</v>
       </c>
       <c r="C10" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+        <v>144</v>
+      </c>
+      <c r="D10" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
+        <v>145</v>
+      </c>
+      <c r="C11" t="s">
+        <v>146</v>
+      </c>
+      <c r="D11" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>314</v>
+      </c>
+      <c r="B12" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B14" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B15" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="B16" t="s">
+        <v>327</v>
+      </c>
+      <c r="C16" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>332</v>
+      </c>
+      <c r="B17" t="s">
+        <v>333</v>
+      </c>
+      <c r="C17" t="s">
+        <v>334</v>
+      </c>
+      <c r="D17" t="s">
+        <v>335</v>
+      </c>
+      <c r="E17" t="s">
+        <v>336</v>
+      </c>
+      <c r="F17" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>167</v>
+        <v>319</v>
+      </c>
+      <c r="B18" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B19" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B20" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B21" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>141</v>
+      </c>
+      <c r="B22" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B23" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B24" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>228</v>
+      </c>
+      <c r="B25" t="s">
+        <v>325</v>
       </c>
     </row>
   </sheetData>
@@ -1824,7 +2278,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9930C30F-55B5-49AC-8A30-AD9CDCECFAFB}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
@@ -1876,7 +2330,7 @@
         <v>13</v>
       </c>
       <c r="D3" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
@@ -1890,7 +2344,7 @@
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
@@ -1904,7 +2358,7 @@
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
@@ -1918,7 +2372,7 @@
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
@@ -1943,10 +2397,10 @@
         <v>9</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="J8" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
@@ -1960,10 +2414,10 @@
         <v>30</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="G9" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
@@ -1977,10 +2431,10 @@
         <v>26</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="G10" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.45">
@@ -1993,11 +2447,11 @@
       <c r="C11" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" t="s">
         <v>25</v>
       </c>
       <c r="G11" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.45">
@@ -2005,7 +2459,7 @@
         <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="C12" t="s">
         <v>31</v>
@@ -2014,7 +2468,7 @@
         <v>33</v>
       </c>
       <c r="G12" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.45">
@@ -2022,12 +2476,12 @@
         <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="C13" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2059,7 +2513,7 @@
         <v>25</v>
       </c>
       <c r="G15" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.45">
@@ -2067,35 +2521,35 @@
         <v>40</v>
       </c>
       <c r="B16" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="B17" t="s">
         <v>41</v>
       </c>
       <c r="G17" t="s">
-        <v>148</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="B18" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2106,604 +2560,814 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF48B9EF-BC37-41C8-953F-9A1246223699}">
-  <dimension ref="A1:H55"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.25" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.25" style="6" customWidth="1"/>
-    <col min="3" max="3" width="96.4140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="96.4140625" customWidth="1"/>
-    <col min="5" max="5" width="65.4140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="69.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="72.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.4140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.25" style="5" customWidth="1"/>
+    <col min="3" max="3" width="76" customWidth="1"/>
+    <col min="4" max="4" width="70.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.6640625" customWidth="1"/>
+    <col min="6" max="6" width="76.83203125" customWidth="1"/>
+    <col min="7" max="7" width="125.08203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>184</v>
+      <c r="A1" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>240</v>
+        <v>207</v>
       </c>
       <c r="D2" t="s">
-        <v>228</v>
+        <v>195</v>
       </c>
       <c r="E2" t="s">
-        <v>221</v>
+        <v>189</v>
       </c>
       <c r="F2" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C3" t="s">
-        <v>238</v>
+        <v>205</v>
       </c>
       <c r="D3" t="s">
-        <v>228</v>
+        <v>195</v>
       </c>
       <c r="E3" t="s">
-        <v>237</v>
+        <v>204</v>
       </c>
       <c r="F3" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C4" t="s">
-        <v>239</v>
+        <v>206</v>
       </c>
       <c r="D4" t="s">
-        <v>228</v>
+        <v>195</v>
       </c>
       <c r="F4" t="s">
-        <v>182</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C5" t="s">
+        <v>261</v>
+      </c>
+      <c r="D5" t="s">
+        <v>195</v>
+      </c>
       <c r="F5" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="3" customFormat="1" ht="8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C6" t="s">
+        <v>278</v>
+      </c>
+      <c r="D6" t="s">
+        <v>279</v>
+      </c>
+      <c r="F6" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A7" s="6" t="s">
+      <c r="B7" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="C7" t="s">
+        <v>280</v>
+      </c>
+      <c r="D7" t="s">
+        <v>281</v>
+      </c>
+      <c r="E7" t="s">
+        <v>282</v>
+      </c>
+      <c r="F7" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B8" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="C8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" t="s">
+        <v>299</v>
+      </c>
+      <c r="E8" t="s">
+        <v>297</v>
+      </c>
+      <c r="F8" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="2" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D7" t="s">
-        <v>227</v>
-      </c>
-      <c r="E7" t="s">
-        <v>220</v>
-      </c>
-      <c r="F7" t="s">
-        <v>186</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="D10" t="s">
+        <v>194</v>
+      </c>
+      <c r="E10" t="s">
+        <v>188</v>
+      </c>
+      <c r="F10" t="s">
+        <v>160</v>
+      </c>
+      <c r="G10" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="C8" t="s">
-        <v>190</v>
-      </c>
-      <c r="E8" t="s">
-        <v>188</v>
-      </c>
-      <c r="F8" t="s">
-        <v>69</v>
-      </c>
-      <c r="G8" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="C9" t="s">
-        <v>191</v>
-      </c>
-      <c r="E9" t="s">
-        <v>187</v>
-      </c>
-      <c r="F9" t="s">
-        <v>185</v>
-      </c>
-      <c r="G9" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" t="s">
-        <v>228</v>
-      </c>
-      <c r="E10" t="s">
-        <v>231</v>
-      </c>
-      <c r="F10" t="s">
-        <v>232</v>
-      </c>
-      <c r="G10" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C11" t="s">
-        <v>233</v>
+        <v>164</v>
       </c>
       <c r="E11" t="s">
+        <v>162</v>
+      </c>
+      <c r="F11" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C12" t="s">
+        <v>165</v>
+      </c>
+      <c r="E12" t="s">
+        <v>161</v>
+      </c>
+      <c r="F12" t="s">
+        <v>159</v>
+      </c>
+      <c r="G12" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>195</v>
+      </c>
+      <c r="E13" t="s">
+        <v>198</v>
+      </c>
+      <c r="F13" t="s">
+        <v>199</v>
+      </c>
+      <c r="G13" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C14" t="s">
+        <v>200</v>
+      </c>
+      <c r="E14" t="s">
+        <v>201</v>
+      </c>
+      <c r="F14" t="s">
+        <v>202</v>
+      </c>
+      <c r="G14" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B15" t="s">
+        <v>208</v>
+      </c>
+      <c r="D15" t="s">
+        <v>231</v>
+      </c>
+      <c r="E15" t="s">
+        <v>263</v>
+      </c>
+      <c r="F15" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s">
+        <v>214</v>
+      </c>
+      <c r="D16" t="s">
+        <v>215</v>
+      </c>
+      <c r="E16" t="s">
+        <v>274</v>
+      </c>
+      <c r="F16" t="s">
+        <v>216</v>
+      </c>
+      <c r="G16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" t="s">
+        <v>266</v>
+      </c>
+      <c r="D17" t="s">
+        <v>290</v>
+      </c>
+      <c r="E17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B18"/>
+      <c r="C18" t="s">
+        <v>289</v>
+      </c>
+      <c r="D18" t="s">
+        <v>291</v>
+      </c>
+      <c r="E18" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B19" t="s">
+        <v>338</v>
+      </c>
+      <c r="C19" t="s">
+        <v>341</v>
+      </c>
+      <c r="D19" t="s">
+        <v>194</v>
+      </c>
+      <c r="E19" t="s">
+        <v>339</v>
+      </c>
+      <c r="F19" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="2" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A21" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" t="s">
+        <v>181</v>
+      </c>
+      <c r="E21" t="s">
+        <v>182</v>
+      </c>
+      <c r="F21" t="s">
+        <v>61</v>
+      </c>
+      <c r="G21" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C22" t="s">
+        <v>268</v>
+      </c>
+      <c r="D22" t="s">
+        <v>184</v>
+      </c>
+      <c r="E22" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" t="s">
+        <v>176</v>
+      </c>
+      <c r="G22" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C23" t="s">
+        <v>269</v>
+      </c>
+      <c r="D23" t="s">
+        <v>183</v>
+      </c>
+      <c r="E23" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C24" t="s">
+        <v>166</v>
+      </c>
+      <c r="D24" t="s">
+        <v>175</v>
+      </c>
+      <c r="E24" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="2" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A26" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" t="s">
+        <v>180</v>
+      </c>
+      <c r="E26" t="s">
+        <v>168</v>
+      </c>
+      <c r="F26" t="s">
+        <v>212</v>
+      </c>
+      <c r="G26" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B27" t="s">
+        <v>122</v>
+      </c>
+      <c r="C27" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F27" t="s">
+        <v>202</v>
+      </c>
+      <c r="G27" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="2" customFormat="1" ht="6.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A29" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" t="s">
+        <v>295</v>
+      </c>
+      <c r="E29" t="s">
+        <v>167</v>
+      </c>
+      <c r="F29" t="s">
+        <v>236</v>
+      </c>
+      <c r="G29" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B30" t="s">
+        <v>172</v>
+      </c>
+      <c r="C30" t="s">
+        <v>191</v>
+      </c>
+      <c r="E30" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B31" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" t="s">
+        <v>192</v>
+      </c>
+      <c r="D31" t="s">
+        <v>168</v>
+      </c>
+      <c r="E31" t="s">
+        <v>168</v>
+      </c>
+      <c r="F31" t="s">
+        <v>210</v>
+      </c>
+      <c r="G31" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" t="s">
+        <v>218</v>
+      </c>
+      <c r="D32" t="s">
+        <v>169</v>
+      </c>
+      <c r="E32" t="s">
+        <v>193</v>
+      </c>
+      <c r="F32" t="s">
         <v>234</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G32" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C33" t="s">
+        <v>219</v>
+      </c>
+      <c r="D33" t="s">
+        <v>170</v>
+      </c>
+      <c r="F33" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C34" t="s">
+        <v>220</v>
+      </c>
+      <c r="D34" t="s">
+        <v>171</v>
+      </c>
+      <c r="E34" t="s">
+        <v>246</v>
+      </c>
+      <c r="F34" t="s">
         <v>235</v>
       </c>
-      <c r="G11" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="3" customFormat="1" ht="8" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A13" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" t="s">
-        <v>211</v>
-      </c>
-      <c r="E13" t="s">
-        <v>212</v>
-      </c>
-      <c r="F13" t="s">
-        <v>75</v>
-      </c>
-      <c r="G13" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A14" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="C14" t="s">
-        <v>214</v>
-      </c>
-      <c r="D14" t="s">
-        <v>216</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="G34" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B35" t="s">
+        <v>53</v>
+      </c>
+      <c r="D35" t="s">
+        <v>250</v>
+      </c>
+      <c r="E35" t="s">
+        <v>253</v>
+      </c>
+      <c r="F35" t="s">
+        <v>349</v>
+      </c>
+      <c r="G35" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B36"/>
+      <c r="C36" t="s">
+        <v>252</v>
+      </c>
+      <c r="D36" t="s">
+        <v>251</v>
+      </c>
+      <c r="E36" t="s">
+        <v>254</v>
+      </c>
+      <c r="F36" t="s">
+        <v>235</v>
+      </c>
+      <c r="G36" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C37" t="s">
+        <v>255</v>
+      </c>
+      <c r="D37" t="s">
+        <v>256</v>
+      </c>
+      <c r="E37" t="s">
+        <v>247</v>
+      </c>
+      <c r="F37" t="s">
+        <v>248</v>
+      </c>
+      <c r="G37" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" s="2" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A39" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" t="s">
+        <v>343</v>
+      </c>
+      <c r="D39" t="s">
+        <v>194</v>
+      </c>
+      <c r="E39" t="s">
+        <v>345</v>
+      </c>
+      <c r="F39" t="s">
+        <v>276</v>
+      </c>
+      <c r="G39" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B40" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="C40" t="s">
+        <v>344</v>
+      </c>
+      <c r="D40" t="s">
         <v>6</v>
       </c>
-      <c r="F14" t="s">
-        <v>205</v>
-      </c>
-      <c r="G14" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="C15" t="s">
-        <v>213</v>
-      </c>
-      <c r="D15" t="s">
-        <v>215</v>
-      </c>
-      <c r="E15" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="C16" t="s">
-        <v>193</v>
-      </c>
-      <c r="D16" t="s">
-        <v>204</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="E40" t="s">
+        <v>346</v>
+      </c>
+      <c r="F40" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" s="2" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A42" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B42" t="s">
+        <v>119</v>
+      </c>
+      <c r="D42" t="s">
+        <v>300</v>
+      </c>
+      <c r="E42" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" s="3" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A18" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C18" t="s">
-        <v>210</v>
-      </c>
-      <c r="E18" t="s">
-        <v>195</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="F42" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B43" t="s">
+        <v>120</v>
+      </c>
+      <c r="D43" t="s">
+        <v>194</v>
+      </c>
+      <c r="E43" t="s">
+        <v>302</v>
+      </c>
+      <c r="F43" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B44" t="s">
+        <v>118</v>
+      </c>
+      <c r="C44" t="s">
+        <v>307</v>
+      </c>
+      <c r="D44" t="s">
+        <v>304</v>
+      </c>
+      <c r="E44" t="s">
+        <v>305</v>
+      </c>
+      <c r="F44" t="s">
+        <v>306</v>
+      </c>
+      <c r="G44" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B45" t="s">
+        <v>310</v>
+      </c>
+      <c r="C45" t="s">
+        <v>311</v>
+      </c>
+      <c r="D45" t="s">
+        <v>194</v>
+      </c>
+      <c r="E45" t="s">
+        <v>309</v>
+      </c>
+      <c r="F45" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" s="2" customFormat="1" ht="4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A46" s="6"/>
+      <c r="B46" s="6"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A47" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C47" t="s">
+        <v>267</v>
+      </c>
+      <c r="E47" t="s">
+        <v>243</v>
+      </c>
+      <c r="F47" t="s">
+        <v>271</v>
+      </c>
+      <c r="G47" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B48" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="C48" t="s">
         <v>245</v>
       </c>
-      <c r="G18" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B19" t="s">
-        <v>143</v>
-      </c>
-      <c r="C19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" t="s">
-        <v>6</v>
-      </c>
-      <c r="F19" t="s">
-        <v>235</v>
-      </c>
-      <c r="G19" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" s="3" customFormat="1" ht="6.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A21" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E21" t="s">
-        <v>194</v>
-      </c>
-      <c r="G21" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B22" t="s">
-        <v>200</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="E48" t="s">
+        <v>270</v>
+      </c>
+      <c r="F48" t="s">
+        <v>271</v>
+      </c>
+      <c r="G48" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" s="2" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A49" s="6"/>
+      <c r="B49" s="6"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A50" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C50" t="s">
+        <v>227</v>
+      </c>
+      <c r="D50" t="s">
+        <v>230</v>
+      </c>
+      <c r="E50" t="s">
         <v>223</v>
       </c>
-      <c r="E22" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B23" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="F50" t="s">
+        <v>222</v>
+      </c>
+      <c r="G50" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="C51" t="s">
+        <v>179</v>
+      </c>
+      <c r="E51" t="s">
         <v>224</v>
       </c>
-      <c r="D23" t="s">
-        <v>195</v>
-      </c>
-      <c r="E23" t="s">
-        <v>195</v>
-      </c>
-      <c r="F23" t="s">
-        <v>243</v>
-      </c>
-      <c r="G23" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B24" t="s">
-        <v>50</v>
-      </c>
-      <c r="C24" t="s">
-        <v>257</v>
-      </c>
-      <c r="D24" t="s">
-        <v>196</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="F51" t="s">
         <v>225</v>
       </c>
-      <c r="G24" t="s">
-        <v>131</v>
-      </c>
-      <c r="H24" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="C25" t="s">
-        <v>258</v>
-      </c>
-      <c r="D25" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="C26" t="s">
-        <v>259</v>
-      </c>
-      <c r="D26" t="s">
-        <v>198</v>
-      </c>
-      <c r="G26" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B27" t="s">
-        <v>58</v>
-      </c>
-      <c r="D27" t="s">
-        <v>202</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="G51" t="s">
         <v>226</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="E28" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" s="3" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A30" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="C30" t="s">
-        <v>248</v>
-      </c>
-      <c r="D30" t="s">
-        <v>249</v>
-      </c>
-      <c r="E30" t="s">
-        <v>252</v>
-      </c>
-      <c r="F30" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B31" t="s">
-        <v>46</v>
-      </c>
-      <c r="C31" t="s">
-        <v>247</v>
-      </c>
-      <c r="D31" t="s">
-        <v>250</v>
-      </c>
-      <c r="E31" t="s">
-        <v>253</v>
-      </c>
-      <c r="F31" t="s">
-        <v>251</v>
-      </c>
-      <c r="G31" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A32" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C32" t="s">
-        <v>71</v>
-      </c>
-      <c r="D32" t="s">
-        <v>256</v>
-      </c>
-      <c r="E32" t="s">
-        <v>72</v>
-      </c>
-      <c r="F32" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A33" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C33" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A34" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C34" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A35" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C35" t="s">
-        <v>56</v>
-      </c>
-      <c r="E35" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A36" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C36" t="s">
-        <v>63</v>
-      </c>
-      <c r="E36" t="s">
-        <v>64</v>
-      </c>
-      <c r="F36" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C37" t="s">
-        <v>60</v>
-      </c>
-      <c r="E37" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C38" t="s">
-        <v>61</v>
-      </c>
-      <c r="E38" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C39" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A40" s="6" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A41" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="C41" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A43" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="C43" t="s">
-        <v>138</v>
-      </c>
-      <c r="D43" t="s">
-        <v>228</v>
-      </c>
-      <c r="E43" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C44" t="s">
-        <v>140</v>
-      </c>
-      <c r="E44" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C45" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="C46" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A47" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="C47" t="s">
-        <v>145</v>
-      </c>
-      <c r="E47" t="s">
-        <v>146</v>
-      </c>
-      <c r="F47" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A48" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="C48" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" s="3" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A51" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="E51" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C52" t="s">
-        <v>208</v>
+        <v>238</v>
+      </c>
+      <c r="D52" t="s">
+        <v>237</v>
+      </c>
+      <c r="E52" t="s">
+        <v>242</v>
+      </c>
+      <c r="F52" t="s">
+        <v>241</v>
       </c>
       <c r="G52" t="s">
-        <v>255</v>
+        <v>232</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="C53" t="s">
-        <v>144</v>
+      <c r="C53" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="D53" t="s">
+        <v>112</v>
+      </c>
+      <c r="E53" t="s">
+        <v>224</v>
+      </c>
+      <c r="F53" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C54" t="s">
-        <v>241</v>
+        <v>259</v>
+      </c>
+      <c r="D54" t="s">
+        <v>257</v>
+      </c>
+      <c r="E54" t="s">
+        <v>258</v>
+      </c>
+      <c r="F54" t="s">
+        <v>260</v>
+      </c>
+      <c r="G54" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="C55" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="D55" s="6"/>
+      <c r="B55" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C55" t="s">
+        <v>294</v>
+      </c>
+      <c r="D55" t="s">
+        <v>285</v>
+      </c>
       <c r="E55" t="s">
-        <v>130</v>
+        <v>286</v>
+      </c>
+      <c r="F55" t="s">
+        <v>287</v>
+      </c>
+      <c r="G55" t="s">
+        <v>288</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Feat] Add Save system, UI
- json으로 세이브 파일을 읽기, 쓰기 가능하게 구현
- UI로 세이브 파일을 선택, 취소 가능함
</commit_message>
<xml_diff>
--- a/Project_Design/Features.xlsx
+++ b/Project_Design/Features.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28926"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/DDFEF73155CF3205/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ttangu\바탕 화면\xrp\Unity\ProjectZ\Project_Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{44B3C5D1-5B15-417F-AA0E-56774807D66A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3FCF5A9-F347-45EA-A27D-44213297ED30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="20" windowWidth="37080" windowHeight="9230" tabRatio="565" firstSheet="4" activeTab="4" xr2:uid="{4CF35248-9F94-4C5D-AC8E-122F6CBF2D14}"/>
+    <workbookView xWindow="1250" yWindow="3310" windowWidth="37150" windowHeight="18290" tabRatio="565" firstSheet="4" activeTab="1" xr2:uid="{4CF35248-9F94-4C5D-AC8E-122F6CBF2D14}"/>
   </bookViews>
   <sheets>
     <sheet name="필요 기능 모음" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="370">
   <si>
     <t>조작 키 (인풋시스템) - C버튼 생략. 다른 키들로 대체함</t>
   </si>
@@ -1456,6 +1456,14 @@
   </si>
   <si>
     <t>수면 복귀 시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데이터는 CSV에서 불러옴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파일은 3개</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1463,7 +1471,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1953,177 +1961,177 @@
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.100000000000001"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.375" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -2138,28 +2146,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A167A73-9D4E-45A5-86A6-04054743346A}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.100000000000001"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="17.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.08203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.875" customWidth="1"/>
+    <col min="6" max="6" width="26.83203125" customWidth="1"/>
     <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -2185,7 +2193,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>43</v>
       </c>
@@ -2193,7 +2201,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>45</v>
       </c>
@@ -2204,12 +2212,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>48</v>
       </c>
@@ -2226,7 +2234,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>50</v>
       </c>
@@ -2243,7 +2251,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>55</v>
       </c>
@@ -2257,7 +2265,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>59</v>
       </c>
@@ -2270,8 +2278,11 @@
       <c r="D10" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="E10" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>63</v>
       </c>
@@ -2282,7 +2293,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>65</v>
       </c>
@@ -2292,8 +2303,11 @@
       <c r="C12" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="D12" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>68</v>
       </c>
@@ -2313,7 +2327,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>74</v>
       </c>
@@ -2321,22 +2335,22 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B17" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>79</v>
       </c>
@@ -2344,12 +2358,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B19" s="8" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>82</v>
       </c>
@@ -2369,7 +2383,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B21" s="8" t="s">
         <v>88</v>
       </c>
@@ -2377,7 +2391,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B22" s="8" t="s">
         <v>90</v>
       </c>
@@ -2385,7 +2399,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B23" s="8" t="s">
         <v>92</v>
       </c>
@@ -2405,7 +2419,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>98</v>
       </c>
@@ -2413,12 +2427,12 @@
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B25" s="9" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>74</v>
       </c>
@@ -2426,7 +2440,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>102</v>
       </c>
@@ -2434,7 +2448,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>104</v>
       </c>
@@ -2456,7 +2470,7 @@
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.100000000000001"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2471,18 +2485,18 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.100000000000001"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="26.5" customWidth="1"/>
     <col min="2" max="2" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>106</v>
       </c>
@@ -2493,7 +2507,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>109</v>
       </c>
@@ -2507,7 +2521,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>112</v>
       </c>
@@ -2521,7 +2535,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>115</v>
       </c>
@@ -2535,7 +2549,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -2549,7 +2563,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>120</v>
       </c>
@@ -2560,7 +2574,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>123</v>
       </c>
@@ -2577,7 +2591,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>127</v>
       </c>
@@ -2594,7 +2608,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>132</v>
       </c>
@@ -2611,7 +2625,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>137</v>
       </c>
@@ -2628,7 +2642,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>142</v>
       </c>
@@ -2645,7 +2659,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>147</v>
       </c>
@@ -2659,7 +2673,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>151</v>
       </c>
@@ -2673,7 +2687,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>155</v>
       </c>
@@ -2690,7 +2704,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>157</v>
       </c>
@@ -2704,7 +2718,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>160</v>
       </c>
@@ -2715,7 +2729,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>163</v>
       </c>
@@ -2736,24 +2750,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF48B9EF-BC37-41C8-953F-9A1246223699}">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.100000000000001"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.25" style="5" customWidth="1"/>
     <col min="3" max="3" width="76" customWidth="1"/>
-    <col min="4" max="4" width="70.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="68.625" customWidth="1"/>
-    <col min="6" max="6" width="76.875" customWidth="1"/>
-    <col min="7" max="7" width="125.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="70.58203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.58203125" customWidth="1"/>
+    <col min="6" max="6" width="76.83203125" customWidth="1"/>
+    <col min="7" max="7" width="125.08203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" thickTop="1" thickBot="1">
+    <row r="1" spans="1:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>166</v>
       </c>
@@ -2776,7 +2790,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="17.45" thickTop="1">
+    <row r="2" spans="1:7" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A2" s="12" t="s">
         <v>173</v>
       </c>
@@ -2793,7 +2807,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C3" t="s">
         <v>178</v>
       </c>
@@ -2807,7 +2821,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C4" t="s">
         <v>181</v>
       </c>
@@ -2818,7 +2832,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
         <v>183</v>
       </c>
@@ -2829,7 +2843,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C6" t="s">
         <v>185</v>
       </c>
@@ -2840,11 +2854,11 @@
         <v>187</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" ht="9" customHeight="1">
+    <row r="7" spans="1:7" s="2" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B8" s="5" t="s">
         <v>188</v>
       </c>
@@ -2861,7 +2875,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B9" s="5" t="s">
         <v>193</v>
       </c>
@@ -2878,11 +2892,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="2" customFormat="1" ht="4.5" customHeight="1">
+    <row r="10" spans="1:7" s="2" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="12" t="s">
         <v>198</v>
       </c>
@@ -2899,7 +2913,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C12" s="11" t="s">
         <v>203</v>
       </c>
@@ -2913,7 +2927,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C13" s="11" t="s">
         <v>207</v>
       </c>
@@ -2927,7 +2941,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C14" s="11" t="s">
         <v>210</v>
       </c>
@@ -2944,7 +2958,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C15" s="11" t="s">
         <v>214</v>
       </c>
@@ -2958,11 +2972,11 @@
         <v>217</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="2" customFormat="1" ht="6.6" customHeight="1">
+    <row r="16" spans="1:7" s="2" customFormat="1" ht="6.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="10" t="s">
         <v>218</v>
       </c>
@@ -2979,7 +2993,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
         <v>223</v>
       </c>
@@ -2999,7 +3013,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
         <v>229</v>
       </c>
@@ -3016,7 +3030,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B20"/>
       <c r="C20" t="s">
         <v>234</v>
@@ -3028,7 +3042,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
         <v>237</v>
       </c>
@@ -3045,11 +3059,11 @@
         <v>240</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="2" customFormat="1" ht="6" customHeight="1">
+    <row r="22" spans="1:7" s="2" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="12" t="s">
         <v>241</v>
       </c>
@@ -3066,7 +3080,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C24" s="11" t="s">
         <v>246</v>
       </c>
@@ -3083,7 +3097,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C25" t="s">
         <v>251</v>
       </c>
@@ -3094,7 +3108,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C26" t="s">
         <v>254</v>
       </c>
@@ -3105,11 +3119,11 @@
         <v>256</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="2" customFormat="1" ht="4.5" customHeight="1">
+    <row r="27" spans="1:7" s="2" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="10" t="s">
         <v>257</v>
       </c>
@@ -3126,7 +3140,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B29" t="s">
         <v>262</v>
       </c>
@@ -3146,11 +3160,11 @@
         <v>263</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="2" customFormat="1" ht="6.6" customHeight="1">
+    <row r="30" spans="1:7" s="2" customFormat="1" ht="6.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="5" t="s">
         <v>264</v>
       </c>
@@ -3167,7 +3181,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B32" t="s">
         <v>269</v>
       </c>
@@ -3178,7 +3192,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B33" t="s">
         <v>272</v>
       </c>
@@ -3198,7 +3212,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B34" t="s">
         <v>276</v>
       </c>
@@ -3218,7 +3232,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C35" t="s">
         <v>282</v>
       </c>
@@ -3229,7 +3243,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C36" t="s">
         <v>284</v>
       </c>
@@ -3246,7 +3260,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B37" t="s">
         <v>289</v>
       </c>
@@ -3263,7 +3277,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B38"/>
       <c r="C38" t="s">
         <v>294</v>
@@ -3281,7 +3295,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C39" t="s">
         <v>298</v>
       </c>
@@ -3298,11 +3312,11 @@
         <v>302</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="2" customFormat="1" ht="6" customHeight="1">
+    <row r="40" spans="1:7" s="2" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="10" t="s">
         <v>303</v>
       </c>
@@ -3322,7 +3336,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B42" s="5" t="s">
         <v>308</v>
       </c>
@@ -3339,11 +3353,11 @@
         <v>306</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="2" customFormat="1" ht="3.95" customHeight="1">
+    <row r="43" spans="1:7" s="2" customFormat="1" ht="4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" s="10" t="s">
         <v>311</v>
       </c>
@@ -3360,12 +3374,12 @@
         <v>315</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B45" s="13" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B46" s="4" t="s">
         <v>317</v>
       </c>
@@ -3382,11 +3396,11 @@
         <v>320</v>
       </c>
     </row>
-    <row r="47" spans="1:7" s="2" customFormat="1" ht="5.0999999999999996" customHeight="1">
+    <row r="47" spans="1:7" s="2" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="7" t="s">
         <v>321</v>
       </c>
@@ -3406,7 +3420,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C49" t="s">
         <v>327</v>
       </c>
@@ -3420,7 +3434,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C50" t="s">
         <v>331</v>
       </c>
@@ -3437,7 +3451,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C51" s="4" t="s">
         <v>336</v>
       </c>
@@ -3451,7 +3465,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C52" t="s">
         <v>339</v>
       </c>
@@ -3468,7 +3482,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B53" s="5" t="s">
         <v>344</v>
       </c>
@@ -3488,7 +3502,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" s="7" t="s">
         <v>350</v>
       </c>
@@ -3505,7 +3519,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B55" t="s">
         <v>355</v>
       </c>
@@ -3519,7 +3533,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B56" t="s">
         <v>358</v>
       </c>
@@ -3539,7 +3553,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B57" t="s">
         <v>364</v>
       </c>

</xml_diff>

<commit_message>
[Feat] Add Save system, UI Manager
- json으로 세이브 파일을 읽기, 쓰기 가능하게 구현
- UI로 세이브 파일을 선택, 취소 가능함
- UI 매니저로 스크립팅 관리. 싱글톤으로 구현
</commit_message>
<xml_diff>
--- a/Project_Design/Features.xlsx
+++ b/Project_Design/Features.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28926"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/DDFEF73155CF3205/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ttangu\바탕 화면\xrp\Unity\ProjectZ\Project_Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{44B3C5D1-5B15-417F-AA0E-56774807D66A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3FCF5A9-F347-45EA-A27D-44213297ED30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="20" windowWidth="37080" windowHeight="9230" tabRatio="565" firstSheet="4" activeTab="4" xr2:uid="{4CF35248-9F94-4C5D-AC8E-122F6CBF2D14}"/>
+    <workbookView xWindow="1250" yWindow="3310" windowWidth="37150" windowHeight="18290" tabRatio="565" firstSheet="4" activeTab="1" xr2:uid="{4CF35248-9F94-4C5D-AC8E-122F6CBF2D14}"/>
   </bookViews>
   <sheets>
     <sheet name="필요 기능 모음" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="370">
   <si>
     <t>조작 키 (인풋시스템) - C버튼 생략. 다른 키들로 대체함</t>
   </si>
@@ -1456,6 +1456,14 @@
   </si>
   <si>
     <t>수면 복귀 시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>데이터는 CSV에서 불러옴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>파일은 3개</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1463,7 +1471,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1953,177 +1961,177 @@
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.100000000000001"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.375" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:1">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:1">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -2138,28 +2146,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A167A73-9D4E-45A5-86A6-04054743346A}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.100000000000001"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="17.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.08203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.875" customWidth="1"/>
+    <col min="6" max="6" width="26.83203125" customWidth="1"/>
     <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -2185,7 +2193,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
         <v>43</v>
       </c>
@@ -2193,7 +2201,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
         <v>45</v>
       </c>
@@ -2204,12 +2212,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>48</v>
       </c>
@@ -2226,7 +2234,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>50</v>
       </c>
@@ -2243,7 +2251,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>55</v>
       </c>
@@ -2257,7 +2265,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>59</v>
       </c>
@@ -2270,8 +2278,11 @@
       <c r="D10" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="E10" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>63</v>
       </c>
@@ -2282,7 +2293,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>65</v>
       </c>
@@ -2292,8 +2303,11 @@
       <c r="C12" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="D12" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>68</v>
       </c>
@@ -2313,7 +2327,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>74</v>
       </c>
@@ -2321,22 +2335,22 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B17" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>79</v>
       </c>
@@ -2344,12 +2358,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B19" s="8" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>82</v>
       </c>
@@ -2369,7 +2383,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B21" s="8" t="s">
         <v>88</v>
       </c>
@@ -2377,7 +2391,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B22" s="8" t="s">
         <v>90</v>
       </c>
@@ -2385,7 +2399,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B23" s="8" t="s">
         <v>92</v>
       </c>
@@ -2405,7 +2419,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>98</v>
       </c>
@@ -2413,12 +2427,12 @@
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B25" s="9" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>74</v>
       </c>
@@ -2426,7 +2440,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>102</v>
       </c>
@@ -2434,7 +2448,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>104</v>
       </c>
@@ -2456,7 +2470,7 @@
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.100000000000001"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2471,18 +2485,18 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.100000000000001"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="26.5" customWidth="1"/>
     <col min="2" max="2" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>106</v>
       </c>
@@ -2493,7 +2507,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>109</v>
       </c>
@@ -2507,7 +2521,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>112</v>
       </c>
@@ -2521,7 +2535,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>115</v>
       </c>
@@ -2535,7 +2549,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -2549,7 +2563,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>120</v>
       </c>
@@ -2560,7 +2574,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>123</v>
       </c>
@@ -2577,7 +2591,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>127</v>
       </c>
@@ -2594,7 +2608,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>132</v>
       </c>
@@ -2611,7 +2625,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>137</v>
       </c>
@@ -2628,7 +2642,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>142</v>
       </c>
@@ -2645,7 +2659,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>147</v>
       </c>
@@ -2659,7 +2673,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>151</v>
       </c>
@@ -2673,7 +2687,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>155</v>
       </c>
@@ -2690,7 +2704,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>157</v>
       </c>
@@ -2704,7 +2718,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>160</v>
       </c>
@@ -2715,7 +2729,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>163</v>
       </c>
@@ -2736,24 +2750,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF48B9EF-BC37-41C8-953F-9A1246223699}">
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.100000000000001"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="17.375" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.25" style="5" customWidth="1"/>
     <col min="3" max="3" width="76" customWidth="1"/>
-    <col min="4" max="4" width="70.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="68.625" customWidth="1"/>
-    <col min="6" max="6" width="76.875" customWidth="1"/>
-    <col min="7" max="7" width="125.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="70.58203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="68.58203125" customWidth="1"/>
+    <col min="6" max="6" width="76.83203125" customWidth="1"/>
+    <col min="7" max="7" width="125.08203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" thickTop="1" thickBot="1">
+    <row r="1" spans="1:7" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>166</v>
       </c>
@@ -2776,7 +2790,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="17.45" thickTop="1">
+    <row r="2" spans="1:7" ht="17.5" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A2" s="12" t="s">
         <v>173</v>
       </c>
@@ -2793,7 +2807,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C3" t="s">
         <v>178</v>
       </c>
@@ -2807,7 +2821,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C4" t="s">
         <v>181</v>
       </c>
@@ -2818,7 +2832,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C5" t="s">
         <v>183</v>
       </c>
@@ -2829,7 +2843,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C6" t="s">
         <v>185</v>
       </c>
@@ -2840,11 +2854,11 @@
         <v>187</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="2" customFormat="1" ht="9" customHeight="1">
+    <row r="7" spans="1:7" s="2" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B8" s="5" t="s">
         <v>188</v>
       </c>
@@ -2861,7 +2875,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B9" s="5" t="s">
         <v>193</v>
       </c>
@@ -2878,11 +2892,11 @@
         <v>197</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="2" customFormat="1" ht="4.5" customHeight="1">
+    <row r="10" spans="1:7" s="2" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="12" t="s">
         <v>198</v>
       </c>
@@ -2899,7 +2913,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C12" s="11" t="s">
         <v>203</v>
       </c>
@@ -2913,7 +2927,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C13" s="11" t="s">
         <v>207</v>
       </c>
@@ -2927,7 +2941,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C14" s="11" t="s">
         <v>210</v>
       </c>
@@ -2944,7 +2958,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C15" s="11" t="s">
         <v>214</v>
       </c>
@@ -2958,11 +2972,11 @@
         <v>217</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="2" customFormat="1" ht="6.6" customHeight="1">
+    <row r="16" spans="1:7" s="2" customFormat="1" ht="6.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="6"/>
       <c r="B16" s="6"/>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="10" t="s">
         <v>218</v>
       </c>
@@ -2979,7 +2993,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
         <v>223</v>
       </c>
@@ -2999,7 +3013,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
         <v>229</v>
       </c>
@@ -3016,7 +3030,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B20"/>
       <c r="C20" t="s">
         <v>234</v>
@@ -3028,7 +3042,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
         <v>237</v>
       </c>
@@ -3045,11 +3059,11 @@
         <v>240</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="2" customFormat="1" ht="6" customHeight="1">
+    <row r="22" spans="1:7" s="2" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="12" t="s">
         <v>241</v>
       </c>
@@ -3066,7 +3080,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C24" s="11" t="s">
         <v>246</v>
       </c>
@@ -3083,7 +3097,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C25" t="s">
         <v>251</v>
       </c>
@@ -3094,7 +3108,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C26" t="s">
         <v>254</v>
       </c>
@@ -3105,11 +3119,11 @@
         <v>256</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="2" customFormat="1" ht="4.5" customHeight="1">
+    <row r="27" spans="1:7" s="2" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="6"/>
       <c r="B27" s="6"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="10" t="s">
         <v>257</v>
       </c>
@@ -3126,7 +3140,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B29" t="s">
         <v>262</v>
       </c>
@@ -3146,11 +3160,11 @@
         <v>263</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="2" customFormat="1" ht="6.6" customHeight="1">
+    <row r="30" spans="1:7" s="2" customFormat="1" ht="6.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="5" t="s">
         <v>264</v>
       </c>
@@ -3167,7 +3181,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B32" t="s">
         <v>269</v>
       </c>
@@ -3178,7 +3192,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B33" t="s">
         <v>272</v>
       </c>
@@ -3198,7 +3212,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B34" t="s">
         <v>276</v>
       </c>
@@ -3218,7 +3232,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C35" t="s">
         <v>282</v>
       </c>
@@ -3229,7 +3243,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C36" t="s">
         <v>284</v>
       </c>
@@ -3246,7 +3260,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B37" t="s">
         <v>289</v>
       </c>
@@ -3263,7 +3277,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B38"/>
       <c r="C38" t="s">
         <v>294</v>
@@ -3281,7 +3295,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C39" t="s">
         <v>298</v>
       </c>
@@ -3298,11 +3312,11 @@
         <v>302</v>
       </c>
     </row>
-    <row r="40" spans="1:7" s="2" customFormat="1" ht="6" customHeight="1">
+    <row r="40" spans="1:7" s="2" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="10" t="s">
         <v>303</v>
       </c>
@@ -3322,7 +3336,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B42" s="5" t="s">
         <v>308</v>
       </c>
@@ -3339,11 +3353,11 @@
         <v>306</v>
       </c>
     </row>
-    <row r="43" spans="1:7" s="2" customFormat="1" ht="3.95" customHeight="1">
+    <row r="43" spans="1:7" s="2" customFormat="1" ht="4" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" s="10" t="s">
         <v>311</v>
       </c>
@@ -3360,12 +3374,12 @@
         <v>315</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B45" s="13" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B46" s="4" t="s">
         <v>317</v>
       </c>
@@ -3382,11 +3396,11 @@
         <v>320</v>
       </c>
     </row>
-    <row r="47" spans="1:7" s="2" customFormat="1" ht="5.0999999999999996" customHeight="1">
+    <row r="47" spans="1:7" s="2" customFormat="1" ht="5.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A47" s="6"/>
       <c r="B47" s="6"/>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="7" t="s">
         <v>321</v>
       </c>
@@ -3406,7 +3420,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C49" t="s">
         <v>327</v>
       </c>
@@ -3420,7 +3434,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C50" t="s">
         <v>331</v>
       </c>
@@ -3437,7 +3451,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C51" s="4" t="s">
         <v>336</v>
       </c>
@@ -3451,7 +3465,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
       <c r="C52" t="s">
         <v>339</v>
       </c>
@@ -3468,7 +3482,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B53" s="5" t="s">
         <v>344</v>
       </c>
@@ -3488,7 +3502,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" s="7" t="s">
         <v>350</v>
       </c>
@@ -3505,7 +3519,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B55" t="s">
         <v>355</v>
       </c>
@@ -3519,7 +3533,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B56" t="s">
         <v>358</v>
       </c>
@@ -3539,7 +3553,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="B57" t="s">
         <v>364</v>
       </c>

</xml_diff>